<commit_message>
add more breakouts. add decoupling cap
</commit_message>
<xml_diff>
--- a/v2/BOM/proto_shield_bom.xlsx
+++ b/v2/BOM/proto_shield_bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Description</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>L1-L18</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>0603 Package</t>
+  </si>
+  <si>
+    <t>GRM188R71C104KA01D</t>
   </si>
 </sst>
 </file>
@@ -106,7 +118,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -168,6 +180,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Museo 700"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
       <name val="Museo 700"/>
     </font>
   </fonts>
@@ -208,7 +226,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -223,6 +241,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -571,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -683,50 +704,52 @@
       <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="10">
+      <c r="A4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="11">
         <v>1</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F4" s="11"/>
       <c r="G4" s="11" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="10" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E5" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="11" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>3</v>
@@ -739,17 +762,29 @@
       <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="10"/>
-      <c r="B6" s="13"/>
+      <c r="A6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="D6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2</v>
+      </c>
       <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="12"/>
+      <c r="G6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>3</v>
+      </c>
       <c r="I6" s="12"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="8"/>
+      <c r="K6" s="6"/>
       <c r="L6" s="7"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
@@ -788,7 +823,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -797,7 +832,7 @@
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="K9" s="8"/>
       <c r="L9" s="7"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
@@ -820,7 +855,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="10"/>
-      <c r="B11" s="13"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -836,7 +871,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -851,38 +886,55 @@
       <c r="N12" s="6"/>
     </row>
     <row r="13" spans="1:14">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="J14"/>
-      <c r="K14"/>
-    </row>
-    <row r="19" spans="7:14" s="1" customFormat="1">
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-    </row>
-    <row r="20" spans="7:14">
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-    </row>
-    <row r="24" spans="7:14">
-      <c r="G24" s="5"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="J15"/>
+      <c r="K15"/>
+    </row>
+    <row r="20" spans="7:14" s="1" customFormat="1">
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="7:14">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+    </row>
+    <row r="25" spans="7:14">
+      <c r="G25" s="5"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H5" r:id="rId1"/>
+    <hyperlink ref="H6" r:id="rId1"/>
     <hyperlink ref="H2" r:id="rId2"/>
     <hyperlink ref="H3" r:id="rId3"/>
-    <hyperlink ref="H4" r:id="rId4"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
clarified wording in the BOM
</commit_message>
<xml_diff>
--- a/v2/BOM/proto_shield_bom.xlsx
+++ b/v2/BOM/proto_shield_bom.xlsx
@@ -51,9 +51,6 @@
     <t>JP1, JP2</t>
   </si>
   <si>
-    <t>0.1" 12-pin header</t>
-  </si>
-  <si>
     <t>68000-412HLF</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>GRM188R71C104KA01D</t>
+  </si>
+  <si>
+    <t>0.1" 12-pin stackable female header</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -617,10 +617,10 @@
         <v>6</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>14</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>0</v>
@@ -629,16 +629,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -647,13 +647,13 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>19</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>7</v>
@@ -677,10 +677,10 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
@@ -705,23 +705,23 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="E4" s="11">
         <v>1</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>3</v>
@@ -735,21 +735,21 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="10">
         <v>1</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>3</v>
@@ -766,18 +766,18 @@
         <v>9</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="D6" s="10" t="s">
-        <v>10</v>
+      <c r="D6" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="E6" s="10">
         <v>2</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>3</v>

</xml_diff>